<commit_message>
fix wrong prefix for emmo
</commit_message>
<xml_diff>
--- a/requests_raw.xlsx
+++ b/requests_raw.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/tto/</t>
+          <t>http://www.w3.org/ns/ssn/systems/</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -469,7 +469,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>https://w3.org/ns/prov#</t>
+          <t>http://xmlns.com/foaf/0.1/</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -485,7 +485,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>http://xmlns.com/foaf/0.1/</t>
+          <t>http://www.w3.org/ns/sosa/</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -493,7 +493,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -501,7 +501,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/glass-ontology/</t>
+          <t>http://purl.org/dc/terms/</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -509,7 +509,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -517,7 +517,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/cpto/</t>
+          <t>http://www.w3.org/ns/oa#</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -533,7 +533,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>https://w3.org/ns/csvw#</t>
+          <t>https://w3id.org/pmd/co/2.0.7/</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -549,7 +549,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/elements/1.1/</t>
+          <t>https://w3.org/ns/csvw#</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -565,7 +565,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/sosa/</t>
+          <t>https://w3.org/ns/prov#</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -581,7 +581,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>http://qudt.org/vocab/unit/</t>
+          <t>http://qudt.org/vocab/quantitykind/</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -597,7 +597,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/oa#</t>
+          <t>http://purl.org/pav/</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -605,7 +605,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/rdf+xml</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -613,7 +613,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>http://purl.org/pav/</t>
+          <t>https://w3id.org/cpto/</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -621,7 +621,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>application/rdf+xml</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -629,7 +629,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/cpto/GGBS/</t>
+          <t>https://w3id.org/pmd/co/</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -645,7 +645,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>http://qudt.org/schema/qudt/</t>
+          <t>https://w3id.org/pmd/tto/</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -661,7 +661,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/co/</t>
+          <t>http://qudt.org/schema/qudt/</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -677,7 +677,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/co/2.0.7/</t>
+          <t>http://swrl.stanford.edu/ontologies/3.3/swrla.owl#</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>application/rdf+xml</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -693,7 +693,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>http://swrl.stanford.edu/ontologies/3.3/swrla.owl#</t>
+          <t>https://w3id.org/pmd/glass-ontology/</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>application/rdf+xml</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -709,7 +709,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/mo/</t>
+          <t>http://www.w3.org/ns/shacl#</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -717,7 +717,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>application/ld+json</t>
+          <t>text/turtle</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -725,7 +725,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>http://qudt.org/vocab/quantitykind/</t>
+          <t>http://purl.org/dc/elements/1.1/</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -741,7 +741,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/ssn/systems/</t>
+          <t>https://w3id.org/cpto/GGBS/</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -749,7 +749,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -757,7 +757,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/</t>
+          <t>http://www.w3.org/ns/prov#</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -773,7 +773,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/prov#</t>
+          <t>https://w3id.org/pmd/mo/</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>text/turtle</t>
+          <t>application/ld+json</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -789,7 +789,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/shacl#</t>
+          <t>http://qudt.org/vocab/unit/</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -805,15 +805,15 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>http://qudt.org/schema/</t>
+          <t>http://nmrML.org/nmrCV#</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>text/html;charset=ISO-8859-1</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -821,7 +821,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>https://qudt.org/2.1/schema/qudt/</t>
+          <t>https://purl.org/bpco/</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -837,15 +837,15 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/2004/02/skos/core#</t>
+          <t>http://purl.obolibrary.org/obo/digitrubber/releases/2023-06-01/</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>application/rdf+xml; qs=0.9</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -853,7 +853,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro/subsets#</t>
+          <t>https://www.tib.eu/digitrubber#</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -869,7 +869,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>https://www.materials.fraunhofer.de/ontologies/</t>
+          <t>http://edamontology.org/</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -877,7 +877,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>application/rdf+xml; charset=utf-8</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -885,7 +885,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/</t>
+          <t>https://doi.org/10.1017/</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html;charset=utf-8</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -901,7 +901,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/chebi/</t>
+          <t>http://www.aidimme.es/</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -909,7 +909,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>text/html;charset=UTF-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -917,15 +917,15 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>http://purl.dataone.org/odo/</t>
+          <t>http://www.w3.org/2004/02/skos/core#</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>application/rdf+xml; qs=0.9</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -933,15 +933,15 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/2003/11/swrl#</t>
+          <t>http://purl.obolibrary.org/obo/ro/docs/reflexivity/</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>406</v>
+        <v>200</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -949,7 +949,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>https://creativecommons.org/licenses/</t>
+          <t>http://www.geneontology.org/formats/oboInOwl#</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -957,7 +957,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -965,11 +965,11 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>https://cmrf.research.uiowa.edu/</t>
+          <t>https://purl.org/bpco#</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -981,15 +981,15 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>https://purl.org/</t>
+          <t>http://purl.allotrope.org/ontologies/</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>200</v>
+        <v>504</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -997,7 +997,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>http://www.geneontology.org/formats/oboInOwl#</t>
+          <t>https://w3id.org/ODE_AM/AMAO#</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1013,15 +1013,15 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>https://www.jeol.co.jp/en/words/emterms/</t>
+          <t>https://doi.org/10.1016/</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/html;charset=utf-8</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -1029,15 +1029,15 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>http://emmo.info/emmo/middle/math#</t>
+          <t>https://w3id.org/okn/o/</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html;charset=UTF-8</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1045,7 +1045,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/WAAMAO/</t>
+          <t>http://www.w3.org/ns/dcat#</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/turtle; charset=utf-8</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -1061,15 +1061,15 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/2000/01/rdf-schema#</t>
+          <t>http://qudt.org/vocab/</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>text/turtle; charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -1077,15 +1077,15 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/MAO/</t>
+          <t>https://gitlab.com/kupferdigital/process-graphs/relaxation-test/</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -1093,15 +1093,15 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>http://www.ontology-of-units-of-measure.org/resource/om-2/</t>
+          <t>https://creativecommons.org/licenses/by-sa/4.0/</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>text/turtle;charset=UTF-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -1109,15 +1109,15 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1007/</t>
+          <t>https://w3id.org/ODE_AM/</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>text/turtle;charset=UTF-8</t>
+          <t>text/html;charset=UTF-8</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1125,15 +1125,15 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/bfo.owl#</t>
+          <t>https://gitlab.com/kupferdigital/process-graphs/tensile-test/</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -1141,15 +1141,15 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>https://www.materialdigital.de/project/</t>
+          <t>https://www.sciencedirect.com/topics/chemistry/electron-diffraction#</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -1157,15 +1157,15 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>https://codebase.helmholtz.cloud/em_glossary/em_glossary/-/blob/main/terms/</t>
+          <t>http://w3id.org/sensotwin/</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -1173,15 +1173,15 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by/</t>
+          <t>https://github.com/oborel/obo-relations/issues/</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -1189,7 +1189,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/digitrubber/</t>
+          <t>http://purl.obolibrary.org/obo/ro/subsets#</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
@@ -1205,15 +1205,15 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>http://ontologydesignpatterns.org/wiki/</t>
+          <t>http://creativecommons.org/licenses/by/</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
@@ -1221,15 +1221,15 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>http://purl.allotrope.org/ontologies/</t>
+          <t>http://wikiba.se/ontology#</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>504</v>
+        <v>200</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
@@ -1237,7 +1237,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/</t>
+          <t>https://cmrf.research.uiowa.edu/</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>text/html;charset=UTF-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
@@ -1253,7 +1253,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>http://material-digital.de/pmdco/</t>
+          <t>https://w3id.org/ODE_AM/AMAO/</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -1269,15 +1269,15 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>http://www.ncbi.nlm.nih.gov/pubmed/</t>
+          <t>http://www.ontology-of-units-of-measure.org/resource/</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html;charset=utf-8</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
@@ -1285,15 +1285,15 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>http://w3id.org/sensotwin/applicationontology/</t>
+          <t>http://purl.obolibrary.org/obo/ro/docs/temporal-semantics/</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
@@ -1301,15 +1301,15 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/2002/07/owl#</t>
+          <t>http://purl.obolibrary.org/obo/bfo/axiom/</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>text/turtle; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
@@ -1317,11 +1317,11 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro/docs/direct-and-indirect-relations/</t>
+          <t>https://gitlab.com/kupferdigital/ontologies/mechanical-testing-ontology/</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1333,7 +1333,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1017/</t>
+          <t>http://w3id.org/sensotwin/applicationontology/</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>text/html;charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
@@ -1349,7 +1349,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>https://orcid.org/</t>
+          <t>https://material-digital.de/pmdco/</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
@@ -1365,15 +1365,15 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/pmd/</t>
+          <t>http://purl.dataone.org/odo/</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>text/html;charset=UTF-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
@@ -1381,7 +1381,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/PBFAO/</t>
+          <t>http://purl.org/dc/</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
@@ -1397,15 +1397,15 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>http://www.ontologyrepository.com/CommonCoreOntologies/</t>
+          <t>https://w3id.org/ODE_AM/CEMAO/</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>application/json; charset=UTF-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
@@ -1413,11 +1413,11 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>http://iirds.tekom.de/iirds#</t>
+          <t>http://purl.obolibrary.org/obo/chebi#</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1429,15 +1429,15 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/ns/dcat#</t>
+          <t>https://doi.org/10.1007/</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>text/turtle; charset=utf-8</t>
+          <t>text/turtle;charset=UTF-8</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
@@ -1445,7 +1445,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro/docs/</t>
+          <t>http://purl.obolibrary.org/obo/bfo.owl#</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
@@ -1461,7 +1461,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/</t>
+          <t>http://purl.obolibrary.org/obo/ro.owl#</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
@@ -1477,7 +1477,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/digitrubber/releases/2023-06-01/</t>
+          <t>https://www.dipromag.de/ottr-templates/</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
@@ -1493,15 +1493,15 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>http://www.ontology-of-units-of-measure.org/resource/</t>
+          <t>http://www.ncbi.nlm.nih.gov/pubmed/</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>text/html;charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
@@ -1509,15 +1509,15 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>http://w3id.org/sensotwin/applicationontology#</t>
+          <t>http://www.w3.org/2000/01/rdf-schema#</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/turtle; charset=utf-8</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
@@ -1525,11 +1525,11 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>https://raw.githubusercontent.com/CommonCoreOntology/CommonCoreOntologies/v2021-03-01/</t>
+          <t>http://emmo.info/emmo/top/annotations#</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -1541,7 +1541,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+          <t>http://www.w3.org/2001/XMLSchema#</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>text/turtle; charset=utf-8</t>
+          <t>application/xml</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -1557,7 +1557,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>https://www.dipromag.de/dipromag_onto/0.1/</t>
+          <t>https://www.globalsino.com/EM/</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -1573,7 +1573,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/</t>
+          <t>https://www.iso.org/obp/ui/</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html;charset=utf-8</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -1589,15 +1589,15 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>https://www.dipromag.de/ottr-templates/</t>
+          <t>http://purl.obolibrary.org/obo/ro/docs/</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -1605,7 +1605,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>http://www.opengis.net/ont/geosparql#</t>
+          <t>http://w3id.org/nfdi4ing/metadata4ing#</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1621,15 +1621,15 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>https://gitlab.com/kupferdigital/ontologies/mechanical-testing-ontology/</t>
+          <t>https://w3id.org/ODE_AM/MAO/</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -1637,15 +1637,15 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/obi-ontology/obi/issues/</t>
+          <t>http://www.referent-tracking.com/_RTU/papers/</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -1653,7 +1653,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/</t>
+          <t>https://www.materialdigital.de/project/</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -1669,7 +1669,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>http://purl.allotrope.org/</t>
+          <t>http://qudt.org/schema/</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/html;charset=ISO-8859-1</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
@@ -1685,7 +1685,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>http://emmo.info/emmo/middle/metrology#</t>
+          <t>http://purl.obolibrary.org/obo/digitrubber/</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
@@ -1701,11 +1701,11 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>http://nmrML.org/nmrCV#</t>
+          <t>http://material-digital.de/pmdco/</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -1717,15 +1717,15 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>http://w3id.org/nfdi4ing/metadata4ing#</t>
+          <t>https://raw.githubusercontent.com/CommonCoreOntology/CommonCoreOntologies/v2021-03-01/</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>text/turtle; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
@@ -1733,7 +1733,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro.owl#</t>
+          <t>https://www.dipromag.de/dipromag_onto/0.1/</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -1749,7 +1749,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>http://wikiba.se/ontology/</t>
+          <t>https://orcid.org/</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
@@ -1765,15 +1765,15 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>https://creativecommons.org/licenses/by-sa/4.0/</t>
+          <t>http://purl.obolibrary.org/obo/</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
@@ -1781,15 +1781,15 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>https://purl.org/bpco/</t>
+          <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/turtle; charset=utf-8</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
@@ -1797,15 +1797,15 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>http://www.aidimme.es/</t>
+          <t>http://www.ontology-of-units-of-measure.org/resource/om-2/</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/turtle;charset=UTF-8</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
@@ -1813,15 +1813,15 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>https://www.iso.org/obp/ui/</t>
+          <t>http://w3id.org/sensotwin/applicationontology#</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>text/html;charset=utf-8</t>
+          <t>text/html; charset=iso-8859-1</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
@@ -1829,15 +1829,15 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>https://gitlab.com/kupferdigital/process-graphs/relaxation-test/</t>
+          <t>http://wikiba.se/ontology/</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
@@ -1845,7 +1845,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>http://emmo.info/emmo/middle/models#</t>
+          <t>http://emmo.info/emmo/middle/math#</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1861,7 +1861,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/AMAO#</t>
+          <t>https://w3id.org/ODE_AM/PBFAO/</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1877,7 +1877,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/bfo/axiom/</t>
+          <t>https://gitlab.com/kupferdigital/process-graphs/lcf-test/</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1893,7 +1893,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>http://www.w3.org/2001/XMLSchema#</t>
+          <t>https://www.materials.fraunhofer.de/ontologies/</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>text/plain</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -1909,7 +1909,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/CEMAO/</t>
+          <t>http://purl.obolibrary.org/obo/ro/docs/direct-and-indirect-relations/</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
@@ -1925,7 +1925,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/ODE_AM/AMAO/</t>
+          <t>https://codebase.helmholtz.cloud/em_glossary/em_glossary/-/blob/main/terms/</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>text/plain; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
@@ -1941,15 +1941,15 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>https://gitlab.com/kupferdigital/process-graphs/tensile-test/</t>
+          <t>http://creativecommons.org/licenses/by/4.0/</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D95" t="inlineStr"/>
@@ -1957,7 +1957,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by/4.0/</t>
+          <t>http://purl.obolibrary.org/obo/chebi/</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html;charset=UTF-8</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -1973,15 +1973,15 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>http://wiki.geneontology.org/index.php/</t>
+          <t>http://emmo.info/emmo/middle/models#</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>200</v>
+        <v>404</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
@@ -1989,11 +1989,11 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>https://gitlab.com/kupferdigital/process-graphs/lcf-test/</t>
+          <t>https://purl.org/</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2005,15 +2005,15 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/chebi#</t>
+          <t>http://wiki.geneontology.org/index.php/</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
@@ -2021,15 +2021,15 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>https://www.tib.eu/digitrubber#</t>
+          <t>https://w3id.org/</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
@@ -2037,15 +2037,15 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/</t>
+          <t>http://www.opengis.net/ont/geosparql#</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>text/html;charset=utf-8</t>
+          <t>text/turtle; charset=utf-8</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
@@ -2053,15 +2053,15 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>https://www.sciencedirect.com/topics/chemistry/electron-diffraction#</t>
+          <t>https://creativecommons.org/licenses/</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>text/html; charset=UTF-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
@@ -2069,7 +2069,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro/docs/temporal-semantics/</t>
+          <t>https://w3id.org/ODE_AM/WAAMAO/</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/plain; charset=utf-8</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
@@ -2085,7 +2085,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>http://emmo.info/emmo/top/annotations#</t>
+          <t>http://emmo.info/emmo/middle/metrology#</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -2101,7 +2101,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>http://edamontology.org/</t>
+          <t>http://ontologydesignpatterns.org/wiki/</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>application/rdf+xml; charset=utf-8</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
@@ -2117,15 +2117,15 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/oborel/obo-relations/issues/</t>
+          <t>http://iirds.tekom.de/iirds#</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>406</v>
+        <v>200</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=utf-8</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
@@ -2133,7 +2133,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>https://www.globalsino.com/EM/</t>
+          <t>http://purl.allotrope.org/</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>text/html</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
@@ -2149,15 +2149,15 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>http://w3id.org/sensotwin/</t>
+          <t>http://www.w3.org/2002/07/owl#</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/turtle; charset=utf-8</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
@@ -2165,15 +2165,15 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>http://www.referent-tracking.com/_RTU/papers/</t>
+          <t>https://w3id.org/pmd/</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>text/html; charset=iso-8859-1</t>
+          <t>text/html;charset=UTF-8</t>
         </is>
       </c>
       <c r="D109" t="inlineStr"/>
@@ -2181,7 +2181,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>https://w3id.org/okn/o/</t>
+          <t>https://en.wikipedia.org/wiki/</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>text/html;charset=UTF-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
@@ -2197,7 +2197,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ro/docs/reflexivity/</t>
+          <t>https://ontobee.org/ontology/</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html; charset=UTF-8</t>
         </is>
       </c>
       <c r="D111" t="inlineStr"/>
@@ -2213,7 +2213,7 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>https://purl.org/bpco#</t>
+          <t>http://www.ontologyrepository.com/CommonCoreOntologies/</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>application/json; charset=UTF-8</t>
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
@@ -2229,7 +2229,7 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>http://wikiba.se/ontology#</t>
+          <t>https://www.jeol.co.jp/en/words/emterms/</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -2245,11 +2245,11 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>http://qudt.org/vocab/</t>
+          <t>http://www.w3.org/2003/11/swrl#</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -2261,15 +2261,15 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>https://material-digital.de/pmdco/</t>
+          <t>https://github.com/obi-ontology/obi/issues/</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>200</v>
+        <v>406</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>text/html; charset=utf-8</t>
+          <t>text/html</t>
         </is>
       </c>
       <c r="D115" t="inlineStr"/>
@@ -2277,112 +2277,114 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>http://www.ebi.ac.uk/efo/</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>'content-type'</t>
-        </is>
-      </c>
+          <t>https://qudt.org/2.1/schema/qudt/</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>404</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>text/html; charset=iso-8859-1</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>http://protege.stanford.edu/plugins/owl/protege#</t>
+          <t>http://org.semanticweb.owlapi/error#</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr">
         <is>
-          <t>'content-type'</t>
+          <t>HTTPConnectionPool(host='org.semanticweb.owlapi', port=80): Max retries exceeded with url: /error (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x00000239D1BFA4B0&gt;: Failed to resolve 'org.semanticweb.owlapi' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>http://org.semanticweb.owlapi/error#</t>
+          <t>http://www.semanticweb.org/ontologies/KnowNow#</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr">
         <is>
-          <t>HTTPConnectionPool(host='org.semanticweb.owlapi', port=80): Max retries exceeded with url: /error (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x000001C822F518B0&gt;: Failed to resolve 'org.semanticweb.owlapi' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>HTTPConnectionPool(host='www.semanticweb.org', port=80): Max retries exceeded with url: /ontologies/KnowNow (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x00000239D1C1FF20&gt;: Failed to resolve 'www.semanticweb.org' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>http://www.semanticweb.org/ontologies/</t>
+          <t>https://glasdigi.cms.uni-jena.de/</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr">
         <is>
-          <t>HTTPConnectionPool(host='www.semanticweb.org', port=80): Max retries exceeded with url: /ontologies/ (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x000001C822F1BA10&gt;: Failed to resolve 'www.semanticweb.org' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>HTTPSConnectionPool(host='glasdigi.cms.uni-jena.de', port=443): Max retries exceeded with url: / (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x00000239D1C1DC10&gt;: Failed to resolve 'glasdigi.cms.uni-jena.de' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>https://glasdigi.cms.uni-jena.de/</t>
+          <t>https://glasdigi.cms.uni-jena.de/glass/</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr">
         <is>
-          <t>HTTPSConnectionPool(host='glasdigi.cms.uni-jena.de', port=443): Max retries exceeded with url: / (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x000001C822F1BA70&gt;: Failed to resolve 'glasdigi.cms.uni-jena.de' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>HTTPSConnectionPool(host='glasdigi.cms.uni-jena.de', port=443): Max retries exceeded with url: /glass/ (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x00000239D1C35520&gt;: Failed to resolve 'glasdigi.cms.uni-jena.de' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>http://www.semanticweb.org/ontologies/KnowNow#</t>
+          <t>http://www.ebi.ac.uk/efo/</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr">
         <is>
-          <t>HTTPConnectionPool(host='www.semanticweb.org', port=80): Max retries exceeded with url: /ontologies/KnowNow (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x000001C822F1ADE0&gt;: Failed to resolve 'www.semanticweb.org' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>'content-type'</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>https://ontobee.org/ontology/</t>
+          <t>http://protege.stanford.edu/plugins/owl/protege#</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr">
         <is>
-          <t>HTTPSConnectionPool(host='ontobee.org', port=443): Max retries exceeded with url: /ontology/ (Caused by ConnectTimeoutError(&lt;urllib3.connection.HTTPSConnection object at 0x000001C822F43920&gt;, 'Connection to ontobee.org timed out. (connect timeout=None)'))</t>
+          <t>'content-type'</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>https://glasdigi.cms.uni-jena.de/glass/</t>
+          <t>http://www.semanticweb.org/ontologies/</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
       <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr">
         <is>
-          <t>HTTPSConnectionPool(host='glasdigi.cms.uni-jena.de', port=443): Max retries exceeded with url: /glass/ (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x000001C822F435F0&gt;: Failed to resolve 'glasdigi.cms.uni-jena.de' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>HTTPConnectionPool(host='www.semanticweb.org', port=80): Max retries exceeded with url: /ontologies/ (Caused by NameResolutionError("&lt;urllib3.connection.HTTPConnection object at 0x00000239D1BF9A60&gt;: Failed to resolve 'www.semanticweb.org' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>

</xml_diff>